<commit_message>
Revert the reverted merge to get the diffs.
This reverts commit 9f64f5a923d15fff9890fa3cc9406ae51cfbfb32, reversing
changes made to efb8c22b638c90f8f9410687f0819199cc4f874a.
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_estimates_csd_by_QUESTION.xlsx
+++ b/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_estimates_csd_by_QUESTION.xlsx
@@ -395,16 +395,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.01086552439795815</v>
+        <v>-0.0653562112283128</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9127557884360062</v>
+        <v>0.5162590491173051</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1844668833093132</v>
+        <v>-0.2635820013437095</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2061979321052295</v>
+        <v>0.1328695788870839</v>
       </c>
     </row>
     <row r="3">
@@ -414,16 +414,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.01725040393772213</v>
+        <v>0.01725040393772195</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9021090095770991</v>
+        <v>0.8934473402079195</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.2589913362128919</v>
+        <v>-0.2364422918969799</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2934921440883362</v>
+        <v>0.2709430997724238</v>
       </c>
     </row>
     <row r="4">
@@ -433,16 +433,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01564798175618947</v>
+        <v>0.01564798175618928</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9111623815778576</v>
+        <v>0.9032937125331343</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2605937583944245</v>
+        <v>-0.2380447140785127</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2918897219068035</v>
+        <v>0.2693406775908912</v>
       </c>
     </row>
     <row r="5">
@@ -452,16 +452,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.009818463971774851</v>
+        <v>0.009818463971774629</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9441874326249829</v>
+        <v>0.9392296143246229</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.2664232761788392</v>
+        <v>-0.2438742318629273</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2860602041223889</v>
+        <v>0.2635111598064765</v>
       </c>
     </row>
     <row r="6">
@@ -471,16 +471,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01161460772199995</v>
+        <v>0.01161460772199954</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9339990249188823</v>
+        <v>0.9281405609428504</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.264627132428614</v>
+        <v>-0.2420780881127023</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2878563478726139</v>
+        <v>0.2653073035567014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>